<commit_message>
update dataset and working env
</commit_message>
<xml_diff>
--- a/Covid dataset/dataset/DeathGlobal.xlsx
+++ b/Covid dataset/dataset/DeathGlobal.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,37 +434,33 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>new_cases</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>150574977</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>new_deaths</t>
         </is>
       </c>
-      <c r="B3" t="n">
-        <v>3180206</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>DeathPercentage</t>
         </is>
       </c>
-      <c r="B4" t="n">
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>150574977</v>
+      </c>
+      <c r="C2" t="n">
+        <v>3180206</v>
+      </c>
+      <c r="D2" t="n">
         <v>2.112041498103633</v>
       </c>
     </row>

</xml_diff>